<commit_message>
Increase the number of anemometer and AQM sensors in the log to 20.
</commit_message>
<xml_diff>
--- a/rack_control/PLC Log format.xlsx
+++ b/rack_control/PLC Log format.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento_dev\rack_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Address</t>
   </si>
@@ -95,126 +95,6 @@
   </si>
   <si>
     <t>IO water level 5</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 0</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 1</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 2</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 3</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 4</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 5</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 6</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 7</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 8</t>
-  </si>
-  <si>
-    <t>Sensor windspeed 9</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 0</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 1</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 2</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 3</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 4</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 5</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 6</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 7</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 8</t>
-  </si>
-  <si>
-    <t>AQM sensor Temperature 9</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 0</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 1</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 2</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 3</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 4</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 5</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 6</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 7</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 8</t>
-  </si>
-  <si>
-    <t>AQM sensor CO2 9</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 0</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 1</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 2</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 3</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 4</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 5</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 6</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 7</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 8</t>
-  </si>
-  <si>
-    <t>AQM sensor Humidity 9</t>
   </si>
   <si>
     <t>Content</t>
@@ -1302,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C13"/>
+  <dimension ref="A3:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1328,8 +1208,9 @@
       <c r="B4">
         <v>10200</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
+      <c r="C4" t="str">
+        <f>CONCATENATE("Sensor windspeed ",A4)</f>
+        <v>Sensor windspeed 0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1341,112 +1222,261 @@
         <f>B4+1</f>
         <v>10201</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
+      <c r="C5" t="str">
+        <f t="shared" ref="C5:C23" si="0">CONCATENATE("Sensor windspeed ",A5)</f>
+        <v>Sensor windspeed 1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" ref="A6:A13" si="0">A5+1</f>
+        <f t="shared" ref="A6:A23" si="1">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B13" si="1">B5+1</f>
+        <f t="shared" ref="B6:B23" si="2">B5+1</f>
         <v>10202</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10203</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10204</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10205</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10206</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10207</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10208</v>
       </c>
-      <c r="C12" t="s">
-        <v>30</v>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10209</v>
       </c>
-      <c r="C13" t="s">
-        <v>31</v>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>10210</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>10211</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>10212</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>10213</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>10214</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>10215</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>10216</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>10217</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>10218</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>10219</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Sensor windspeed 19</v>
       </c>
     </row>
   </sheetData>
@@ -1456,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C32"/>
+  <dimension ref="A2:C62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1482,8 +1512,9 @@
       <c r="B3">
         <v>10300</v>
       </c>
-      <c r="C3" t="s">
-        <v>32</v>
+      <c r="C3" t="str">
+        <f>CONCATENATE("AQM sensor Temperature ",A3)</f>
+        <v>AQM sensor Temperature 0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1495,376 +1526,826 @@
         <f>B3+1</f>
         <v>10301</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C22" si="0">CONCATENATE("AQM sensor Temperature ",A4)</f>
+        <v>AQM sensor Temperature 1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A12" si="0">A4+1</f>
+        <f t="shared" ref="A5:A62" si="1">A4+1</f>
         <v>2</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B12" si="1">B4+1</f>
+        <f t="shared" ref="B5:B62" si="2">B4+1</f>
         <v>10302</v>
       </c>
-      <c r="C5" t="s">
-        <v>34</v>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10303</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10304</v>
       </c>
-      <c r="C7" t="s">
-        <v>36</v>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10305</v>
       </c>
-      <c r="C8" t="s">
-        <v>37</v>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10306</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10307</v>
       </c>
-      <c r="C10" t="s">
-        <v>39</v>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10308</v>
       </c>
-      <c r="C11" t="s">
-        <v>40</v>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10309</v>
       </c>
-      <c r="C12" t="s">
-        <v>41</v>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" ref="A13" si="2">A12+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13" si="3">B12+1</f>
+        <f t="shared" si="2"/>
         <v>10310</v>
       </c>
-      <c r="C13" t="s">
-        <v>42</v>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" ref="A14:A21" si="4">A13+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B21" si="5">B13+1</f>
+        <f t="shared" si="2"/>
         <v>10311</v>
       </c>
-      <c r="C14" t="s">
-        <v>43</v>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10312</v>
       </c>
-      <c r="C15" t="s">
-        <v>44</v>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10313</v>
       </c>
-      <c r="C16" t="s">
-        <v>45</v>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10314</v>
       </c>
-      <c r="C17" t="s">
-        <v>46</v>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10315</v>
       </c>
-      <c r="C18" t="s">
-        <v>47</v>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10316</v>
       </c>
-      <c r="C19" t="s">
-        <v>48</v>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10317</v>
       </c>
-      <c r="C20" t="s">
-        <v>49</v>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10318</v>
       </c>
-      <c r="C21" t="s">
-        <v>50</v>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" ref="A22" si="6">A21+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22" si="7">B21+1</f>
+        <f t="shared" si="2"/>
         <v>10319</v>
       </c>
-      <c r="C22" t="s">
-        <v>51</v>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>AQM sensor Temperature 19</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" ref="A23" si="8">A22+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23" si="9">B22+1</f>
+        <f t="shared" si="2"/>
         <v>10320</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
+      <c r="C23" t="str">
+        <f>CONCATENATE("AQM sensor CO2 ",A23-20)</f>
+        <v>AQM sensor CO2 0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" ref="A24:A32" si="10">A23+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:B32" si="11">B23+1</f>
+        <f t="shared" si="2"/>
         <v>10321</v>
       </c>
-      <c r="C24" t="s">
-        <v>53</v>
+      <c r="C24" t="str">
+        <f t="shared" ref="C24:C42" si="3">CONCATENATE("AQM sensor CO2 ",A24-20)</f>
+        <v>AQM sensor CO2 1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10322</v>
       </c>
-      <c r="C25" t="s">
-        <v>54</v>
+      <c r="C25" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10323</v>
       </c>
-      <c r="C26" t="s">
-        <v>55</v>
+      <c r="C26" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10324</v>
       </c>
-      <c r="C27" t="s">
-        <v>56</v>
+      <c r="C27" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10325</v>
       </c>
-      <c r="C28" t="s">
-        <v>57</v>
+      <c r="C28" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10326</v>
       </c>
-      <c r="C29" t="s">
-        <v>58</v>
+      <c r="C29" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10327</v>
       </c>
-      <c r="C30" t="s">
-        <v>59</v>
+      <c r="C30" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10328</v>
       </c>
-      <c r="C31" t="s">
-        <v>60</v>
+      <c r="C31" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10329</v>
       </c>
-      <c r="C32" t="s">
-        <v>61</v>
+      <c r="C32" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="2"/>
+        <v>10330</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="2"/>
+        <v>10331</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="2"/>
+        <v>10332</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>10333</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>10334</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
+        <v>10335</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
+        <v>10336</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>10337</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>10338</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="2"/>
+        <v>10339</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="3"/>
+        <v>AQM sensor CO2 19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="2"/>
+        <v>10340</v>
+      </c>
+      <c r="C43" t="str">
+        <f>CONCATENATE("AQM sensor Humidity ",A43-40)</f>
+        <v>AQM sensor Humidity 0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="2"/>
+        <v>10341</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" ref="C44:C62" si="4">CONCATENATE("AQM sensor Humidity ",A44-40)</f>
+        <v>AQM sensor Humidity 1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="2"/>
+        <v>10342</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="2"/>
+        <v>10343</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="2"/>
+        <v>10344</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="2"/>
+        <v>10345</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="2"/>
+        <v>10346</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="2"/>
+        <v>10347</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="2"/>
+        <v>10348</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="2"/>
+        <v>10349</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="2"/>
+        <v>10350</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="2"/>
+        <v>10351</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="2"/>
+        <v>10352</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="2"/>
+        <v>10353</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="2"/>
+        <v>10354</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="2"/>
+        <v>10355</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="2"/>
+        <v>10356</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="2"/>
+        <v>10357</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="2"/>
+        <v>10358</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="2"/>
+        <v>10359</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="4"/>
+        <v>AQM sensor Humidity 19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1886,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2317,7 +2798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -2329,7 +2810,7 @@
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -2337,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
@@ -2346,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -2355,7 +2836,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
@@ -2364,7 +2845,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
@@ -2373,7 +2854,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
@@ -2382,7 +2863,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
@@ -2391,7 +2872,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
@@ -2400,7 +2881,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -2409,7 +2890,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
@@ -2418,7 +2899,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
@@ -2427,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
@@ -2436,7 +2917,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
@@ -2445,7 +2926,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -2454,7 +2935,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
@@ -2463,7 +2944,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
@@ -2472,7 +2953,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -2481,7 +2962,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
@@ -2490,7 +2971,7 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
@@ -2499,7 +2980,7 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -2508,7 +2989,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
@@ -2517,7 +2998,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
@@ -2526,7 +3007,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
@@ -2535,7 +3016,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
@@ -2543,7 +3024,7 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
@@ -2551,7 +3032,7 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
@@ -2559,7 +3040,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
@@ -2567,7 +3048,7 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
@@ -2575,7 +3056,7 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
@@ -2583,7 +3064,7 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>